<commit_message>
bare essentials for creating work
</commit_message>
<xml_diff>
--- a/data-files/OutExcel4.xlsx
+++ b/data-files/OutExcel4.xlsx
@@ -402,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -438,28 +438,28 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lep62vrw.hfvm</v>
+        <v>lgqy9rb3-0bmn</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-02-28T22:10:00</v>
+        <v>2023-04-21T14:34:06.217</v>
       </c>
       <c r="C2" t="str">
-        <v>lep62vrw</v>
+        <v>lgqy9rbd</v>
       </c>
       <c r="D2" t="str">
         <v>FALSE</v>
       </c>
       <c r="E2" t="str">
-        <v>doae</v>
+        <v>0m7w</v>
       </c>
       <c r="F2" t="str">
-        <v>Event</v>
+        <v>test one</v>
       </c>
       <c r="G2" t="str">
-        <v>🧪</v>
+        <v>1️⃣</v>
       </c>
       <c r="H2" t="str">
-        <v>A test definition, for plain events</v>
+        <v>Initial desc</v>
       </c>
       <c r="I2" t="str">
         <v>SECOND</v>
@@ -467,43 +467,101 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lep62vpsx.doqd</v>
+        <v>lgqy9rbd-avpc</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-03-12T22:10:00</v>
+        <v>2023-04-21T14:34:06.217</v>
       </c>
       <c r="C3" t="str">
-        <v>lep62vrw</v>
+        <v>lgqy9rbe</v>
       </c>
       <c r="D3" t="str">
         <v>FALSE</v>
       </c>
       <c r="E3" t="str">
-        <v>seae</v>
+        <v>ay7l</v>
       </c>
       <c r="F3" t="str">
-        <v>Movie</v>
+        <v>twooo</v>
       </c>
       <c r="G3" t="str">
         <v>2️⃣</v>
       </c>
       <c r="H3" t="str">
-        <v>A 2nd definition, with two points</v>
+        <v>now with a description</v>
       </c>
       <c r="I3" t="str">
+        <v>WEEK</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>lgqy9rbe-2ban</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2023-04-21T14:34:06.218</v>
+      </c>
+      <c r="C4" t="str">
+        <v>lgqy9rbe</v>
+      </c>
+      <c r="D4" t="str">
+        <v>FALSE</v>
+      </c>
+      <c r="E4" t="str">
+        <v>05a8</v>
+      </c>
+      <c r="F4" t="str">
+        <v>afree</v>
+      </c>
+      <c r="G4" t="str">
+        <v>3️⃣</v>
+      </c>
+      <c r="H4" t="str">
+        <v>Set a description</v>
+      </c>
+      <c r="I4" t="str">
+        <v>SECOND</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>lgqy9rbe-0keb</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2023-04-21T14:34:06.218</v>
+      </c>
+      <c r="C5" t="str">
+        <v>lgqy9rbe</v>
+      </c>
+      <c r="D5" t="str">
+        <v>FALSE</v>
+      </c>
+      <c r="E5" t="str">
+        <v>e0bq</v>
+      </c>
+      <c r="F5" t="str">
+        <v>FOUR</v>
+      </c>
+      <c r="G5" t="str">
+        <v>4️⃣</v>
+      </c>
+      <c r="H5" t="str">
+        <v>having fun</v>
+      </c>
+      <c r="I5" t="str">
         <v>SECOND</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -548,121 +606,83 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>lep65ghw.rghw</v>
+        <v>lgqy9rbe-0bcq</v>
       </c>
       <c r="B2" t="str">
-        <v>2023-04-21T12:36:54.274</v>
+        <v>2023-04-21T14:34:06.218</v>
       </c>
       <c r="C2" t="str">
-        <v>lep62vrw</v>
+        <v>lgqy9rbe</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="str">
-        <v>doae</v>
+        <v>e0bq</v>
       </c>
       <c r="F2" t="str">
-        <v>apox</v>
+        <v>0pc6</v>
       </c>
       <c r="G2" t="str">
-        <v>Event</v>
+        <v>set alternatively</v>
       </c>
       <c r="H2" t="str">
-        <v>🏷️</v>
+        <v>☝️</v>
       </c>
       <c r="I2" t="str">
-        <v>The main text for the event</v>
+        <v>Set a description</v>
       </c>
       <c r="J2" t="str">
-        <v>TEXT</v>
+        <v>BOOL</v>
       </c>
       <c r="K2" t="str">
         <v>COUNT</v>
       </c>
       <c r="L2" t="str">
-        <v>MARKDOWN</v>
+        <v>TEXT</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>lep65gcy.rghw</v>
+        <v>lgqy9rbe-3tnn</v>
       </c>
       <c r="B3" t="str">
-        <v>2023-03-12T22:10:00</v>
+        <v>2023-04-21T14:34:06.218</v>
       </c>
       <c r="C3" t="str">
-        <v>lep62vrw</v>
+        <v>lgqy9rbe</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
       <c r="E3" t="str">
-        <v>seae</v>
+        <v>e0bq</v>
       </c>
       <c r="F3" t="str">
-        <v>oese</v>
+        <v>0tb7</v>
       </c>
       <c r="G3" t="str">
-        <v>Title</v>
+        <v>test point</v>
       </c>
       <c r="H3" t="str">
-        <v>🎬</v>
+        <v>🆕</v>
       </c>
       <c r="I3" t="str">
-        <v>The name of hte movie</v>
+        <v>Set a description</v>
       </c>
       <c r="J3" t="str">
         <v>TEXT</v>
       </c>
       <c r="K3" t="str">
-        <v>COUNTUNIQUE</v>
+        <v>COUNT</v>
       </c>
       <c r="L3" t="str">
         <v>TEXT</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>lep65g3sq.fipe</v>
-      </c>
-      <c r="B4" t="str">
-        <v>2023-03-12T22:10:00</v>
-      </c>
-      <c r="C4" t="str">
-        <v>lep62vrw</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="str">
-        <v>seae</v>
-      </c>
-      <c r="F4" t="str">
-        <v>momm</v>
-      </c>
-      <c r="G4" t="str">
-        <v>First time?</v>
-      </c>
-      <c r="H4" t="str">
-        <v>🎍</v>
-      </c>
-      <c r="I4" t="str">
-        <v>Have you seen this before?</v>
-      </c>
-      <c r="J4" t="str">
-        <v>BOOL</v>
-      </c>
-      <c r="K4" t="str">
-        <v>COUNTOFEACH</v>
-      </c>
-      <c r="L4" t="str">
-        <v>YESNO</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L3"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>